<commit_message>
Fixed LHS sampling to only sample across uncertainties (X) that vary (Ls still vary for all Ls) and rebuilt templates with PFLO:ALL_NO_STOPPING_DEFORESTATION_PLUR
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_se_calibrated.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-0" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5004" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5008" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5007" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5009" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2644,4 +2645,309 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9600000000000001</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9199999999999999</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8200000000000001</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.6799999999999999</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.6599999999999999</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.5800000000000001</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
version used to run experiment 'sisepuede_run_2023-10-08T02:22:14.745372'
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_se_calibrated.xlsx
@@ -11,6 +11,11 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5004" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5007" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5009" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5011" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5012" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5013" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5014" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5015" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2950,4 +2955,1529 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.9829063213546697</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9658126427093395</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9487189640640092</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.931625285418679</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9145316067733488</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.8974379281280185</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.8803442494826883</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.863250570837358</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8461568921920278</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.8290632135466975</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.8119695349013674</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.7948758562560371</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.7777821776107068</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.7606884989653766</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.7435948203200462</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.726501141674716</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.7094074630293857</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.6923137843840557</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.6752201057387253</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.6581264270933951</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.6410327484480649</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.6239390698027346</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.6068453911574043</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.5897517125120741</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.5726580338667439</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.9862304763364699</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9724609526729397</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9586914290094095</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9449219053458794</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9311523816823493</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.9173828580188191</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.903613334355289</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.8898438106917588</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8760742870282288</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.8623047633646985</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.8485352397011684</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.8347657160376383</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.820996192374108</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.8072266687105779</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.7934571450470478</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.7796876213835175</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.7659180977199874</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.7521485740564573</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.7383790503929272</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.724609526729397</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.7108400030658669</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.6970704794023368</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.6833009557388066</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.6695314320752765</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.6557619084117463</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.9831702487644064</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9663404975288129</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9495107462932192</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9326809950576255</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.915851243822032</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.8990214925864384</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.8821917413508448</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.8653619901152512</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8485322388796576</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.831702487644064</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.8148727364084704</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.7980429851728768</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.7812132339372831</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.7643834827016895</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.7475537314660958</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.7307239802305022</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.7138942289949086</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.6970644777593151</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.6802347265237214</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.6634049752881279</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.6465752240525343</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.6297454728169407</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.6129157215813471</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.5960859703457535</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.5792562191101598</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.9888585559026216</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9777171118052433</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.966575667707865</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9554342236104866</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.9442927795131083</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.9331513354157299</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.9220098913183516</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.9108684472209733</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.899727003123595</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.8885855590262166</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.8774441149288383</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.86630267083146</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.8551612267340816</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.8440197826367033</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.8328783385393249</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.8217368944419465</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.8105954503445683</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.79945400624719</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.7883125621498116</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.7771711180524332</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.7660296739550549</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.7548882298576767</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.7437467857602983</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.7326053416629199</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.7214638975655416</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AS2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subsector</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>variable</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>normalize_group</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>trajgroup_no_vary_q</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>uniform_scaling_q</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>variable_trajectory_group_trajectory_type</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>max_35</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>min_35</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG1" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS1" s="1" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>frac_gnrl_eating_red_meat</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>1</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.9813124864730004</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.9626249729460008</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.9439374594190011</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9252499458920015</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.906562432365002</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.8878749188380024</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.8691874053110027</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.8504998917840031</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.8318123782570036</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.813124864730004</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.7944373512030043</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.7757498376760047</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.7570623241490051</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.7383748106220054</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.7196872970950059</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.7009997835680062</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.6823122700410066</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.663624756514007</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.6449372429870075</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.6262497294600078</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.6075622159330083</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.5888747024060086</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.5701871888790091</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.5514996753520094</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.5328121618250098</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added input_base_all_sectors.csv for version control and included new templates for baseline
</commit_message>
<xml_diff>
--- a/ref/ingestion/calibrated/argentina/model_input_variables_argentina_se_calibrated.xlsx
+++ b/ref/ingestion/calibrated/argentina/model_input_variables_argentina_se_calibrated.xlsx
@@ -11,11 +11,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5004" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5007" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5009" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5011" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5012" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5013" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5014" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="strategy_id-5015" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1131,7 +1126,9 @@
           <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>13</v>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -2222,7 +2219,9 @@
           <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>13</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -2527,7 +2526,9 @@
           <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>13</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -2832,7 +2833,9 @@
           <t>frac_gnrl_eating_red_meat</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>13</v>
+      </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
@@ -2955,1529 +2958,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subsector</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>normalize_group</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>trajgroup_no_vary_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group_trajectory_type</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>max_35</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>min_35</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>frac_gnrl_eating_red_meat</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.9829063213546697</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.9658126427093395</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.9487189640640092</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.931625285418679</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.9145316067733488</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.8974379281280185</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.8803442494826883</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.863250570837358</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.8461568921920278</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.8290632135466975</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0.8119695349013674</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.7948758562560371</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.7777821776107068</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0.7606884989653766</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.7435948203200462</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.726501141674716</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.7094074630293857</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.6923137843840557</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.6752201057387253</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.6581264270933951</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.6410327484480649</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.6239390698027346</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.6068453911574043</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.5897517125120741</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.5726580338667439</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subsector</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>normalize_group</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>trajgroup_no_vary_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group_trajectory_type</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>max_35</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>min_35</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>frac_gnrl_eating_red_meat</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.9862304763364699</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.9724609526729397</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.9586914290094095</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.9449219053458794</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.9311523816823493</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.9173828580188191</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.903613334355289</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.8898438106917588</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.8760742870282288</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.8623047633646985</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0.8485352397011684</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.8347657160376383</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.820996192374108</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0.8072266687105779</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.7934571450470478</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.7796876213835175</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.7659180977199874</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.7521485740564573</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.7383790503929272</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.724609526729397</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.7108400030658669</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.6970704794023368</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.6833009557388066</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.6695314320752765</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.6557619084117463</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subsector</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>normalize_group</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>trajgroup_no_vary_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group_trajectory_type</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>max_35</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>min_35</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>frac_gnrl_eating_red_meat</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.9831702487644064</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.9663404975288129</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.9495107462932192</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.9326809950576255</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.915851243822032</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.8990214925864384</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.8821917413508448</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.8653619901152512</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.8485322388796576</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.831702487644064</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0.8148727364084704</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.7980429851728768</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.7812132339372831</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0.7643834827016895</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.7475537314660958</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.7307239802305022</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.7138942289949086</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.6970644777593151</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.6802347265237214</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.6634049752881279</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.6465752240525343</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.6297454728169407</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.6129157215813471</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.5960859703457535</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.5792562191101598</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subsector</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>normalize_group</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>trajgroup_no_vary_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group_trajectory_type</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>max_35</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>min_35</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>frac_gnrl_eating_red_meat</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.9888585559026216</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.9777171118052433</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.966575667707865</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.9554342236104866</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.9442927795131083</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.9331513354157299</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.9220098913183516</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.9108684472209733</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.899727003123595</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.8885855590262166</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0.8774441149288383</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.86630267083146</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.8551612267340816</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0.8440197826367033</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.8328783385393249</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.8217368944419465</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.8105954503445683</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.79945400624719</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.7883125621498116</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.7771711180524332</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.7660296739550549</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.7548882298576767</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.7437467857602983</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.7326053416629199</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.7214638975655416</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AS2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subsector</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>normalize_group</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>trajgroup_no_vary_q</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>uniform_scaling_q</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>variable_trajectory_group_trajectory_type</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>max_35</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>min_35</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M1" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N1" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="O1" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="AD1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="AE1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="AF1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG1" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="AH1" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="AI1" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AJ1" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AK1" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AM1" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AN1" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="AO1" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="AR1" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="AS1" s="1" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>frac_gnrl_eating_red_meat</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1</v>
-      </c>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.9813124864730004</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.9626249729460008</v>
-      </c>
-      <c r="W2" t="n">
-        <v>0.9439374594190011</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.9252499458920015</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.906562432365002</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.8878749188380024</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.8691874053110027</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.8504998917840031</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.8318123782570036</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.813124864730004</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0.7944373512030043</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.7757498376760047</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.7570623241490051</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0.7383748106220054</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.7196872970950059</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.7009997835680062</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.6823122700410066</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.663624756514007</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.6449372429870075</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.6262497294600078</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.6075622159330083</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>0.5888747024060086</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.5701871888790091</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>0.5514996753520094</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0.5328121618250098</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>